<commit_message>
LoadFileInQueue and Test file are added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1575,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2695,8 +2694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
InvoiceProcessing_Dispatcher has been created
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1574,8 +1574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2694,7 +2694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>